<commit_message>
fix typo 3.57 -> 3.75
</commit_message>
<xml_diff>
--- a/notebooks/shiptype_database/DTV_shiptypes_database.xlsx
+++ b/notebooks/shiptype_database/DTV_shiptypes_database.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\11205224_DigitalTwin_Vaarwegcorridor\Input_shipping_classes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/baart_f/src/digitaltwin-waterway/notebooks/shiptype_database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBBFFD25-50F3-4D3D-B7A1-DF3B7BF806A1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6D3D57D-490C-2643-9A0B-6A1D93764758}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="420" windowWidth="25440" windowHeight="15390" xr2:uid="{1ED1099D-4BC9-49B6-B1CA-AFE2C82F23A7}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20020" xr2:uid="{1ED1099D-4BC9-49B6-B1CA-AFE2C82F23A7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -783,30 +783,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA60D031-48D8-4F7A-9139-CD0C7ED9F83A}">
   <dimension ref="A1:S34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="46.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="13" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="46.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="24.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.33203125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="18" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="24.83203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="26.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>64</v>
       </c>
@@ -865,7 +865,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>0</v>
       </c>
@@ -918,7 +918,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -977,7 +977,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -1036,7 +1036,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -1095,7 +1095,7 @@
         <v>796</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -1154,7 +1154,7 @@
         <v>951</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -1213,7 +1213,7 @@
         <v>1171</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>54</v>
       </c>
@@ -1272,7 +1272,7 @@
         <v>1497</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>54</v>
       </c>
@@ -1331,7 +1331,7 @@
         <v>2026</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -1390,7 +1390,7 @@
         <v>2689</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -1449,7 +1449,7 @@
         <v>3900</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1508,7 +1508,7 @@
         <v>3932</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -1567,7 +1567,7 @@
         <v>5186</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -1626,7 +1626,7 @@
         <v>5900</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -1685,7 +1685,7 @@
         <v>740</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>0</v>
       </c>
@@ -1744,7 +1744,7 @@
         <v>761</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>5</v>
       </c>
@@ -1803,7 +1803,7 @@
         <v>1806</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>8</v>
       </c>
@@ -1847,7 +1847,7 @@
         <v>3.5</v>
       </c>
       <c r="O18">
-        <v>3.57</v>
+        <v>3.75</v>
       </c>
       <c r="P18">
         <v>1.5</v>
@@ -1862,7 +1862,7 @@
         <v>5236</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>11</v>
       </c>
@@ -1921,7 +1921,7 @@
         <v>2260</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>11</v>
       </c>
@@ -1980,7 +1980,7 @@
         <v>5454</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>16</v>
       </c>
@@ -2039,7 +2039,7 @@
         <v>8145</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>0</v>
       </c>
@@ -2098,7 +2098,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>20</v>
       </c>
@@ -2157,7 +2157,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>21</v>
       </c>
@@ -2216,7 +2216,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>22</v>
       </c>
@@ -2275,7 +2275,7 @@
         <v>946</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>23</v>
       </c>
@@ -2334,7 +2334,7 @@
         <v>1478</v>
       </c>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -2393,7 +2393,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -2437,7 +2437,7 @@
         <v>6.02</v>
       </c>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>26</v>
       </c>
@@ -2481,7 +2481,7 @@
         <v>6.02</v>
       </c>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>8</v>
       </c>
@@ -2540,7 +2540,7 @@
         <v>5495</v>
       </c>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>11</v>
       </c>
@@ -2599,7 +2599,7 @@
         <v>5601</v>
       </c>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>16</v>
       </c>
@@ -2658,7 +2658,7 @@
         <v>11186</v>
       </c>
     </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>38</v>
       </c>
@@ -2717,7 +2717,7 @@
         <v>16493</v>
       </c>
     </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>41</v>
       </c>

</xml_diff>